<commit_message>
DAY-3 Events , Loop and Conditional Rendering
</commit_message>
<xml_diff>
--- a/Training Plan_React JS_40 Hrs.xlsx
+++ b/Training Plan_React JS_40 Hrs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepakkumarshinde/Documents/teaching/broadridge/React JS-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F097862D-821A-6343-A1C4-B1F0B4DC6EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37189E7E-4236-6D47-A06B-11CCE832C17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BC91FDED-9C10-4469-86A6-FD3E956DFB10}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{BC91FDED-9C10-4469-86A6-FD3E956DFB10}"/>
   </bookViews>
   <sheets>
     <sheet name="React JS" sheetId="1" r:id="rId1"/>
@@ -346,69 +346,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Event Handling:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-•	Handling events in React
-•	Synthetic events
-•	Passing arguments to event handlers
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Conditional Rendering:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-•	Using if-else statements
-•	Conditional rendering with ternary operators
-•	Short-circuit evaluation
-Lists and Keys:
-•	Rendering lists in React
-•	Using the map function
-•	Importance of keys in lists
-•	Dynamic lists
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Hands-On: Todo list with add/remove</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>Context API &amp; Styling</t>
     </r>
     <r>
@@ -1157,6 +1094,249 @@
         <family val="2"/>
       </rPr>
       <t>Hands-On: Counter app with props &amp; state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Event Handling:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Handling events in React</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Synthetic events</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Passing arguments to event handlers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Conditional Rendering:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Using if-else statements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Conditional rendering with ternary operators</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Short-circuit evaluation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Lists and Keys:
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Rendering lists in React</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Using the map function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Importance of keys in lists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+•	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Dynamic lists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Hands-On: Todo list with add/remove</t>
     </r>
   </si>
 </sst>
@@ -1483,6 +1663,9 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1521,9 +1704,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1861,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875AA830-E690-44C6-8147-E87AB6E11114}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D11" zoomScale="225" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D6" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1877,24 +2057,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1927,11 +2107,11 @@
       <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>45</v>
+      <c r="E4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="13" customFormat="1" ht="195" x14ac:dyDescent="0.2">
@@ -1943,12 +2123,12 @@
         <v>9</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="36"/>
+        <v>56</v>
+      </c>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1" ht="255" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
@@ -1959,13 +2139,13 @@
         <v>9</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>46</v>
+        <v>57</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="180" x14ac:dyDescent="0.2">
@@ -1977,12 +2157,12 @@
         <v>9</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="26"/>
+        <v>37</v>
+      </c>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:6" s="13" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
@@ -1996,10 +2176,10 @@
         <v>16</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1" ht="195" x14ac:dyDescent="0.2">
@@ -2011,12 +2191,12 @@
         <v>9</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="26"/>
+        <v>39</v>
+      </c>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" s="13" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
@@ -2030,10 +2210,10 @@
         <v>14</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1" ht="165" x14ac:dyDescent="0.2">
@@ -2045,12 +2225,12 @@
         <v>9</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="26"/>
+        <v>41</v>
+      </c>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" s="13" customFormat="1" ht="165" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
@@ -2061,12 +2241,12 @@
         <v>9</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="27"/>
+        <v>42</v>
+      </c>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
@@ -2077,12 +2257,12 @@
         <v>9</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="F13" s="29"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D14" s="4"/>
@@ -2126,7 +2306,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -2134,37 +2314,37 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="11" t="s">
         <v>31</v>
       </c>

</xml_diff>